<commit_message>
Included description to Scripts and Images for Readme.md
</commit_message>
<xml_diff>
--- a/1_Custom electronics for automated monitoring/Hardware/RPi power_budget_storage calculations.xlsx
+++ b/1_Custom electronics for automated monitoring/Hardware/RPi power_budget_storage calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpou\Desktop\git-chapter3\1_Custom electronics for automated monitoring\Calculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpou\Desktop\git-chapter3\1_Custom electronics for automated monitoring\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743565D6-3A02-4205-8414-CCE25AA72EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A030EEF-7078-4ABB-8067-7CFFDD869801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power consumption" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>mpou:</t>
         </r>
@@ -60,7 +60,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Rpi zero = 1,2W
@@ -76,7 +76,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>mpou:</t>
         </r>
@@ -85,7 +85,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 (this is *2 because: 1- the need of recharge the battery while 2- powering the system)</t>
@@ -110,7 +110,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>mpou:</t>
         </r>
@@ -119,7 +119,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 number of months</t>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="117">
   <si>
     <t>Rpi 4B+</t>
   </si>
@@ -337,18 +337,12 @@
     <t>https://www.amazon.es/AZDelivery-Puente-Jumper-juegos-cables/dp/B074P726ZR/ref=sr_1_2_sspa?keywords=jumper%2Bwire&amp;qid=1644571670&amp;s=industrial&amp;sprefix=jumper%2Cindustrial%2C107&amp;sr=1-2-spons&amp;smid=A1X7QLRQH87QA3&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzOVY1RDBSS1dLTDRCJmVuY3J5cHRlZElkPUEwNzA3MDAzMjAwSENPRjlPVDhSNyZlbmNyeXB0ZWRBZElkPUEwNDA3NDU4MVlQQkRINlFMTERMWCZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU&amp;th=1</t>
   </si>
   <si>
-    <t>HDMI-microHDMI adaptor</t>
-  </si>
-  <si>
     <t>USB 4G Dongle</t>
   </si>
   <si>
     <t>https://www.amazon.es/Huawei-HE8372B-E8372/dp/B0179R5X30/ref=sr_1_13?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=29ZOONVO6C59W&amp;keywords=usb+dongle+sim&amp;qid=1641982654&amp;sprefix=usb+dongle+sim%2Caps%2C110&amp;sr=8-13</t>
   </si>
   <si>
-    <t>HDMI-miniHDMI adaptor</t>
-  </si>
-  <si>
     <t>Movistar</t>
   </si>
   <si>
@@ -367,15 +361,9 @@
     <t>Strong black wide tape</t>
   </si>
   <si>
-    <t>Brico Sant Celoni</t>
-  </si>
-  <si>
     <t>Metalic grippers</t>
   </si>
   <si>
-    <t>U nails</t>
-  </si>
-  <si>
     <t>Solar panel 190W</t>
   </si>
   <si>
@@ -491,6 +479,9 @@
   </si>
   <si>
     <t>Number of systems</t>
+  </si>
+  <si>
+    <t>Local shop</t>
   </si>
 </sst>
 </file>
@@ -500,11 +491,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -576,14 +574,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -698,84 +696,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,10 +785,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -997,7 +987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F985"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1014,7 +1004,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1044,7 +1034,7 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <f>((B3*B4*B6+C3*C4*B6+D3*D4*24)/B8)*1.2</f>
         <v>66.7</v>
       </c>
@@ -1076,7 +1066,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <f>E3*B7</f>
         <v>133.4</v>
       </c>
@@ -1110,7 +1100,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <f>E3*2*B8/(B10*B9)</f>
         <v>285.85714285714289</v>
       </c>
@@ -1138,7 +1128,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <f>E9/B8</f>
         <v>23.821428571428573</v>
       </c>
@@ -2135,7 +2125,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2190,7 +2180,7 @@
         <v>61200</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -2220,7 +2210,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -2253,17 +2243,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.5546875" customWidth="1"/>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.21875" customWidth="1"/>
   </cols>
@@ -2279,911 +2269,901 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>48.65</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <v>1</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="23">
         <f t="shared" ref="G4:G33" si="0">E4*F4</f>
         <v>48.65</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="22">
         <v>6.95</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="20">
         <f>F4</f>
         <v>1</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="23">
         <f t="shared" si="0"/>
         <v>6.95</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="22">
         <v>16.899999999999999</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="20">
         <v>13</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="23">
         <f t="shared" si="0"/>
         <v>219.7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="22">
         <v>1.45</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="20">
         <f>F6</f>
         <v>13</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="23">
         <f t="shared" si="0"/>
         <v>18.849999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="22">
         <v>4.95</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="20">
         <f>F6</f>
         <v>13</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="23">
         <f t="shared" si="0"/>
         <v>64.350000000000009</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="26" t="s">
+      <c r="A9" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" s="24">
+      <c r="D9" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="22">
         <v>13.1</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="20">
         <v>1</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="23">
         <f t="shared" si="0"/>
         <v>13.1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="22">
         <v>15</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="20">
         <f>F4+F6</f>
         <v>14</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="23">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="22">
         <v>69.58</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="20">
         <f>F4</f>
         <v>1</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="23">
         <f t="shared" si="0"/>
         <v>69.58</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="22">
         <v>17.989999999999998</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="20">
         <f>F4+F6</f>
         <v>14</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="23">
         <f t="shared" si="0"/>
         <v>251.85999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="18" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="27" t="s">
+    <row r="13" spans="1:7" s="16" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="27">
         <v>2.35</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="25">
         <f>F4</f>
         <v>1</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="28">
         <f t="shared" si="0"/>
         <v>2.35</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="22">
         <v>3.98</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="20">
         <f>F6</f>
         <v>13</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="23">
         <f t="shared" si="0"/>
         <v>51.74</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="24">
+      <c r="D15" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="22">
         <v>12.99</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="20">
         <v>3</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="23">
         <f t="shared" si="0"/>
         <v>38.97</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="22">
         <f>11.53/10</f>
         <v>1.153</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="20">
         <f>F12</f>
         <v>14</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="23">
         <f t="shared" si="0"/>
         <v>16.141999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="23" t="s">
+      <c r="C17" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="22">
         <v>5.89</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="20">
         <v>1</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="23">
         <f t="shared" si="0"/>
         <v>5.89</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="22">
         <v>6.49</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="20">
         <v>2</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="23">
         <f t="shared" si="0"/>
         <v>12.98</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="24">
+      <c r="E19" s="22">
         <v>64.95</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="20">
         <f>F4</f>
         <v>1</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="23">
         <f t="shared" si="0"/>
         <v>64.95</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="24">
+      <c r="C20" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="22">
         <v>28</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="20">
         <v>4</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="23">
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="24">
+      <c r="C21" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="22">
         <v>159.99</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="20">
         <v>1</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="23">
         <f t="shared" si="0"/>
         <v>159.99</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="24">
+      <c r="D22" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="22">
         <v>154.88</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="20">
         <v>1</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="23">
         <f t="shared" ref="G22" si="1">E22*F22</f>
         <v>154.88</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="22" t="s">
+      <c r="A23" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="24">
+      <c r="C23" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="22">
         <v>1</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="20">
         <v>2</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="23">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="22" t="s">
+      <c r="A24" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="24">
+      <c r="D24" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="22">
         <v>224.99</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="20">
         <v>1</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="23">
         <f t="shared" si="0"/>
         <v>224.99</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="22" t="s">
+    <row r="25" spans="1:7" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="24">
+      <c r="D25" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="22">
         <v>98.35</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="20">
         <v>1</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="30">
         <f>E25*F25</f>
         <v>98.35</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E26" s="24">
+      <c r="D26" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="22">
         <v>44.09</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="20">
         <v>1</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="30">
         <f t="shared" ref="G26" si="2">E26*F26</f>
         <v>44.09</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="22" t="s">
+      <c r="A27" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="24">
+      <c r="D27" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="22">
         <f>15.99/3</f>
         <v>5.33</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="20">
         <v>3</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="23">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="22" t="s">
+      <c r="A28" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="24">
+      <c r="D28" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="22">
         <f>14.99/5</f>
         <v>2.9980000000000002</v>
       </c>
-      <c r="F28" s="22">
+      <c r="F28" s="20">
         <v>5</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="23">
         <f t="shared" si="0"/>
         <v>14.990000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="22" t="s">
+      <c r="A29" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="24">
+      <c r="D29" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="22">
         <f>25.99/30</f>
         <v>0.86633333333333329</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="20">
         <v>30</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="23">
         <f t="shared" si="0"/>
         <v>25.99</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" s="33" t="s">
+    <row r="30" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="35">
+      <c r="D30" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="22">
         <f>12.52/10</f>
         <v>1.252</v>
       </c>
-      <c r="F30" s="33">
+      <c r="F30" s="20">
         <f>F6+F4</f>
         <v>14</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="23">
         <f t="shared" si="0"/>
         <v>17.527999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="33" t="s">
+    <row r="31" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="35">
+      <c r="D31" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="22">
         <v>14.86</v>
       </c>
-      <c r="F31" s="33">
+      <c r="F31" s="20">
         <v>1</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="23">
         <f t="shared" si="0"/>
         <v>14.86</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="36" t="s">
+      <c r="A32" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" s="35">
+      <c r="D32" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="22">
         <v>18.399999999999999</v>
       </c>
-      <c r="F32" s="33">
+      <c r="F32" s="20">
         <v>1</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="23">
         <f t="shared" si="0"/>
         <v>18.399999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="22" t="s">
+      <c r="A33" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="24">
+      <c r="D33" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="22">
         <v>8.9</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F33" s="29">
         <v>1</v>
       </c>
-      <c r="G33" s="41">
+      <c r="G33" s="36">
         <f t="shared" si="0"/>
         <v>8.9</v>
       </c>
     </row>
     <row r="34" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E34" s="12"/>
-      <c r="G34" s="42">
+      <c r="E34" s="11"/>
+      <c r="G34" s="37">
         <f>SUM(G4:G32)</f>
         <v>2000.1200000000001</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E35" s="12"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="43">
+      <c r="A37" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="44">
+      <c r="B38" s="39">
         <f>B37*G34</f>
         <v>2000.1200000000001</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="17"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="15"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E42" s="12"/>
+      <c r="E42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E43" s="12"/>
+      <c r="E43" s="11"/>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="36">
         <v>49.99</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="12">
+      <c r="C45" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="36">
         <f>7.5/2</f>
         <v>3.75</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="12"/>
+      <c r="A46" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" s="36">
+        <v>30.99</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="12"/>
-    </row>
-    <row r="48" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E48" s="12">
-        <v>30.99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E49" s="12">
+      <c r="A47" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="36">
         <v>4.2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="E50" s="12"/>
-    </row>
+    <row r="48" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" s="36">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E49" s="37">
+        <f>SUM(E44:E48)</f>
+        <v>97.13000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E51" s="12">
-        <v>1.95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E52" s="12">
-        <v>8.1999999999999993</v>
-      </c>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="E51" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3203,7 +3183,7 @@
     <hyperlink ref="D19" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
     <hyperlink ref="D21" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
     <hyperlink ref="D24" r:id="rId16" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="D52" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="D48" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
     <hyperlink ref="D27" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
     <hyperlink ref="D28" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
     <hyperlink ref="D29" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000015000000}"/>

</xml_diff>